<commit_message>
Now we have a working implemetation
</commit_message>
<xml_diff>
--- a/resource/params_values_shen.xlsx
+++ b/resource/params_values_shen.xlsx
@@ -190,10 +190,10 @@
     <t xml:space="preserve">mapreduce.map.memory.mb</t>
   </si>
   <si>
-    <t xml:space="preserve">1024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">819, 922, 1126, 1228</t>
+    <t xml:space="preserve">4096</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2048, 3072, 5120, 6144</t>
   </si>
   <si>
     <t xml:space="preserve">mapreduce.map.output.compress</t>
@@ -263,10 +263,10 @@
     <t xml:space="preserve">mapreduce.reduce.memory.mb</t>
   </si>
   <si>
-    <t xml:space="preserve">2048</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1638, 1843, 2253, 2458</t>
+    <t xml:space="preserve">8192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4096, 6144, 10240, 12288</t>
   </si>
   <si>
     <t xml:space="preserve">mapreduce.reduce.merge.inmem.threshold</t>
@@ -954,9 +954,6 @@
     <t xml:space="preserve">yarn.scheduler.maximum-allocation-mb</t>
   </si>
   <si>
-    <t xml:space="preserve">8192</t>
-  </si>
-  <si>
     <t xml:space="preserve">yarn.scheduler.maximum-allocation-vcores</t>
   </si>
   <si>
@@ -967,6 +964,9 @@
   </si>
   <si>
     <t xml:space="preserve">yarn.scheduler.minimum-allocation-mb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1638, 1843, 2253, 2458</t>
   </si>
   <si>
     <t xml:space="preserve">yarn.scheduler.minimum-allocation-vcores</t>
@@ -1140,9 +1140,9 @@
   <dimension ref="A1:F129"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F45" activeCellId="0" sqref="F45"/>
+      <selection pane="bottomLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2961,7 +2961,7 @@
         <v>290</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C115" s="2" t="s">
         <v>40</v>
@@ -3065,7 +3065,7 @@
         <v>301</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>302</v>
+        <v>79</v>
       </c>
       <c r="C123" s="2" t="s">
         <v>169</v>
@@ -3075,26 +3075,26 @@
     </row>
     <row r="124" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="B124" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="C124" s="2" t="s">
         <v>304</v>
-      </c>
-      <c r="C124" s="2" t="s">
-        <v>305</v>
       </c>
       <c r="E124" s="0"/>
       <c r="F124" s="0"/>
     </row>
     <row r="125" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B125" s="0" t="n">
         <v>2048</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>80</v>
+        <v>306</v>
       </c>
       <c r="E125" s="0"/>
       <c r="F125" s="0"/>

</xml_diff>